<commit_message>
updated ssid txt to md
</commit_message>
<xml_diff>
--- a/Default-SSID-Keyspace&Length.xlsx
+++ b/Default-SSID-Keyspace&Length.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hayde\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hayde\Documents\GitHub\Hash-Cracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA46AF5-D9FC-45B5-BF9C-CF6A58A2E91D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B3DC5E-C1B1-42E1-9380-0C354558BA6B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6648" xr2:uid="{C1B36B05-07CD-4EB0-886C-7B2D7651E369}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="187">
   <si>
     <t>[0-9a-f]</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Len: 10</t>
   </si>
   <si>
-    <t>BTHomeHub-XXXX</t>
-  </si>
-  <si>
     <t>[2-9a-f]</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>ONOXXXX</t>
   </si>
   <si>
-    <t>DJAWEB_#####</t>
-  </si>
-  <si>
     <t>TIM_PN51T_XXXX</t>
   </si>
   <si>
@@ -192,9 +186,6 @@
     <t>UPCXXXXXXX</t>
   </si>
   <si>
-    <t>SKYXXXXX</t>
-  </si>
-  <si>
     <t>Tech_XXXXXXXX</t>
   </si>
   <si>
@@ -291,9 +282,6 @@
     <t>BOLT!SUPER 4G-XXXX</t>
   </si>
   <si>
-    <t>4 numbers + Last 4 of SSID</t>
-  </si>
-  <si>
     <t>3 words, with hyphens in-between.</t>
   </si>
   <si>
@@ -360,9 +348,6 @@
     <t>Sitecom_XXXX</t>
   </si>
   <si>
-    <t>http://www.ph-mb.com/products/sky-calc</t>
-  </si>
-  <si>
     <t>SpeedTouchXXXXXX</t>
   </si>
   <si>
@@ -547,6 +532,60 @@
   </si>
   <si>
     <t>Default pasword is the MAC address</t>
+  </si>
+  <si>
+    <t>BTHomeHub1-XXXX</t>
+  </si>
+  <si>
+    <t>MyCharterWiFi-XX</t>
+  </si>
+  <si>
+    <t>[Adjective + Noun + 1 or 3 Digits]</t>
+  </si>
+  <si>
+    <t>MyCSpectrumWiFi-XX</t>
+  </si>
+  <si>
+    <t>Len:Varies</t>
+  </si>
+  <si>
+    <t>SKYXXXXX (Sky Q Hub)</t>
+  </si>
+  <si>
+    <t>[BCDFLMNPQRSTVWXY]</t>
+  </si>
+  <si>
+    <t>SKYXXXXX (Sky Hub)</t>
+  </si>
+  <si>
+    <t>http://www.ph-mb.com/products/sky-calc  First hex value in SSID -&gt; Last letter of PSK, X: 0 = P,1 = Q,2 = R,3 = S,4 = T,5 = N,6 = V,7 = W,8 = X,9 = Y,A = L,B = B,C = C,D = D,E = M,F = F</t>
+  </si>
+  <si>
+    <t>DJAWEB_xxxxx</t>
+  </si>
+  <si>
+    <t>(Broken Algo)</t>
+  </si>
+  <si>
+    <t>7aac</t>
+  </si>
+  <si>
+    <t>bfd3</t>
+  </si>
+  <si>
+    <t>fbff</t>
+  </si>
+  <si>
+    <t>9a1e</t>
+  </si>
+  <si>
+    <t>491a</t>
+  </si>
+  <si>
+    <t>01ec</t>
+  </si>
+  <si>
+    <t>4 numbers + Last 4 of SSID ?H?H?H?H</t>
   </si>
 </sst>
 </file>
@@ -698,12 +737,6 @@
   <dxfs count="7">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -765,6 +798,12 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -779,16 +818,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{509E80FE-156B-42A3-BD60-719245CDDEC3}" name="Table1" displayName="Table1" ref="A1:D121" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{509E80FE-156B-42A3-BD60-719245CDDEC3}" name="Table1" displayName="Table1" ref="A1:D121" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A1:D121" xr:uid="{176D8D76-6912-4C7A-9987-EBCB4E86C46C}"/>
   <sortState ref="A2:D121">
     <sortCondition ref="A1:A121"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{75121D7B-775F-486F-BEA4-A798993D99D1}" name="SSID" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{81AD25E5-6241-4141-BAE4-D95F0C3B2827}" name="Keyspace" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{B997D3FC-9526-442C-A433-1CE024231467}" name="Length" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{14B4AA29-A0C9-4611-8885-B2C8945DBEFD}" name="Notes" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{75121D7B-775F-486F-BEA4-A798993D99D1}" name="SSID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{81AD25E5-6241-4141-BAE4-D95F0C3B2827}" name="Keyspace" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B997D3FC-9526-442C-A433-1CE024231467}" name="Length" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{14B4AA29-A0C9-4611-8885-B2C8945DBEFD}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1093,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04B4ED97-2274-474F-9E77-207F43F3A69D}">
   <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="D67" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1107,24 +1146,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -1133,74 +1172,74 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>1</v>
@@ -1209,10 +1248,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1</v>
@@ -1221,82 +1260,82 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>1</v>
@@ -1305,52 +1344,52 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>88</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
-        <v>23</v>
+        <v>169</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>1</v>
@@ -1359,10 +1398,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>1</v>
@@ -1371,10 +1410,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>1</v>
@@ -1383,10 +1422,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>1</v>
@@ -1395,10 +1434,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>1</v>
@@ -1407,60 +1446,60 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3" t="s">
-        <v>43</v>
+        <v>178</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>1</v>
@@ -1469,106 +1508,106 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>1</v>
@@ -1577,394 +1616,392 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="3" t="s">
-        <v>103</v>
+        <v>170</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1</v>
+        <v>173</v>
       </c>
       <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="3" t="s">
-        <v>47</v>
+        <v>172</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>13</v>
+        <v>171</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>155</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="3" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>170</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D49" s="4"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="3" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D51" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="3" t="s">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="9" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D53" s="11"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>140</v>
+        <v>4</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="D54" s="4"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="3" t="s">
-        <v>107</v>
+        <v>49</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>108</v>
+        <v>11</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="D55" s="4"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="3" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>5</v>
+        <v>135</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="D56" s="4"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>127</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D57" s="4"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="3" t="s">
-        <v>110</v>
+        <v>27</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D58" s="4"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="3" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="3" t="s">
-        <v>172</v>
+        <v>106</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>173</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D60" s="4"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="3" t="s">
-        <v>112</v>
+        <v>176</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D61" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="3" t="s">
-        <v>52</v>
+        <v>174</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>113</v>
+        <v>175</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D62" s="4"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="3" t="s">
-        <v>36</v>
+        <v>167</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="3" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="3" t="s">
-        <v>114</v>
+        <v>50</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>5</v>
+        <v>108</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D65" s="4"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>171</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="3" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>1</v>
@@ -1973,33 +2010,35 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>143</v>
+        <v>69</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="3" t="s">
-        <v>116</v>
+        <v>38</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D70" s="4"/>
+      <c r="D70" s="4" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="9" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>0</v>
@@ -2011,24 +2050,24 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="3" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>6</v>
+        <v>137</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>45</v>
+        <v>14</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>1</v>
@@ -2037,260 +2076,280 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D74" s="6" t="s">
-        <v>153</v>
-      </c>
+      <c r="D74" s="4"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="3" t="s">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D75" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="3" t="s">
-        <v>35</v>
+        <v>112</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D76" s="4"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="3" t="s">
-        <v>132</v>
+        <v>36</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>133</v>
+        <v>4</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>147</v>
+        <v>1</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="3" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>131</v>
+        <v>5</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>146</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D78" s="4"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="3" t="s">
-        <v>119</v>
+        <v>34</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>164</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D79" s="4"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="3" t="s">
-        <v>54</v>
+        <v>127</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D80" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="3" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>6</v>
+        <v>126</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>165</v>
+        <v>3</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="3" t="s">
-        <v>58</v>
+        <v>114</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D82" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="3" t="s">
-        <v>120</v>
+        <v>52</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>158</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D83" s="4"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>160</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D85" s="4"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="3" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="3" t="s">
-        <v>121</v>
+        <v>58</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D88" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="3" t="s">
-        <v>134</v>
+        <v>56</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="9" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>125</v>
+        <v>77</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="D91" s="4"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" s="3"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="4"/>
+      <c r="A92" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" s="3"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="4"/>
+      <c r="A93" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" s="3"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
+      <c r="A94" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="D94" s="4"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2336,37 +2395,49 @@
       <c r="D101" s="4"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" s="3"/>
+      <c r="A102" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="4"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" s="3"/>
+      <c r="A103" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="4"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104" s="3"/>
+      <c r="A104" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="4"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" s="3"/>
+      <c r="A105" s="3" t="s">
+        <v>183</v>
+      </c>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="4"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" s="3"/>
+      <c r="A106" s="3" t="s">
+        <v>184</v>
+      </c>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="4"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="3"/>
+      <c r="A107" s="3" t="s">
+        <v>185</v>
+      </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="4"/>
@@ -2457,15 +2528,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D69" r:id="rId1" xr:uid="{8703070F-DB6C-4011-BA8C-675845111056}"/>
+    <hyperlink ref="D72" r:id="rId1" xr:uid="{8703070F-DB6C-4011-BA8C-675845111056}"/>
     <hyperlink ref="D44" r:id="rId2" xr:uid="{54EA4967-DAFB-4160-B907-5FEE0425D980}"/>
-    <hyperlink ref="D74" r:id="rId3" xr:uid="{1C516D04-1975-4CD6-9122-BA71D56AE92E}"/>
+    <hyperlink ref="D77" r:id="rId3" xr:uid="{1C516D04-1975-4CD6-9122-BA71D56AE92E}"/>
     <hyperlink ref="D17" r:id="rId4" xr:uid="{5A742AA0-664B-4A85-A46E-8C1D801FCC28}"/>
+    <hyperlink ref="D61" r:id="rId5" xr:uid="{FC2B0BAB-F319-48D1-8785-4DE97084903B}"/>
+    <hyperlink ref="D81" r:id="rId6" location="64032" xr:uid="{8FADCFDF-8DB0-4542-9908-DC47ADD90C25}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>